<commit_message>
add data to problems types
</commit_message>
<xml_diff>
--- a/excel_files/problems_types.xlsx
+++ b/excel_files/problems_types.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="20">
   <si>
     <t>type</t>
   </si>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A15" sqref="A15:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +436,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -458,7 +458,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -469,7 +469,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -588,9 +588,169 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
       <c r="C17" s="1">
-        <v>20</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="1">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>